<commit_message>
update trans progress xls
</commit_message>
<xml_diff>
--- a/games/dqm2/translation-progress.xlsx
+++ b/games/dqm2/translation-progress.xlsx
@@ -62,7 +62,7 @@
     <t>Field 61 - 65</t>
   </si>
   <si>
-    <t>62-65已收回</t>
+    <t>Field 66 - 70</t>
   </si>
 </sst>
 </file>
@@ -393,7 +393,7 @@
     <xf numFmtId="1" fontId="5" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1799,7 +1799,7 @@
     <row r="11" ht="20.35" customHeight="1">
       <c r="A11" s="18"/>
       <c r="B11" s="19"/>
-      <c r="C11" s="14"/>
+      <c r="C11" s="16"/>
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
@@ -1812,8 +1812,8 @@
       <c r="B12" s="12">
         <v>9527</v>
       </c>
-      <c r="C12" t="s" s="20">
-        <v>16</v>
+      <c r="C12" t="s" s="9">
+        <v>5</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="14"/>
@@ -1821,9 +1821,13 @@
       <c r="G12" s="14"/>
     </row>
     <row r="13" ht="20.35" customHeight="1">
-      <c r="A13" s="18"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="14"/>
+      <c r="A13" t="s" s="11">
+        <v>16</v>
+      </c>
+      <c r="B13" s="12">
+        <v>9527</v>
+      </c>
+      <c r="C13" s="20"/>
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>

</xml_diff>

<commit_message>
update dispatch Field 51 - 55 to zhuzi
</commit_message>
<xml_diff>
--- a/games/dqm2/translation-progress.xlsx
+++ b/games/dqm2/translation-progress.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
   <si>
     <t>表格 1</t>
   </si>
@@ -60,6 +60,15 @@
   </si>
   <si>
     <t>Demo 31- 36</t>
+  </si>
+  <si>
+    <t>Field 1 - 50</t>
+  </si>
+  <si>
+    <t>小智分配</t>
+  </si>
+  <si>
+    <t>Field 51 - 55</t>
   </si>
   <si>
     <t>Field 61 - 65</t>
@@ -1659,7 +1668,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1810,9 +1819,13 @@
       <c r="G10" s="14"/>
     </row>
     <row r="11" ht="20.35" customHeight="1">
-      <c r="A11" s="19"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="17"/>
+      <c r="A11" t="s" s="11">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s" s="16">
+        <v>17</v>
+      </c>
+      <c r="C11" s="14"/>
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
@@ -1820,14 +1833,12 @@
     </row>
     <row r="12" ht="20.35" customHeight="1">
       <c r="A12" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="B12" s="12">
-        <v>9527</v>
-      </c>
-      <c r="C12" t="s" s="9">
-        <v>5</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="B12" t="s" s="8">
+        <v>4</v>
+      </c>
+      <c r="C12" s="17"/>
       <c r="D12" s="14"/>
       <c r="E12" s="14"/>
       <c r="F12" s="14"/>
@@ -1835,12 +1846,14 @@
     </row>
     <row r="13" ht="20.35" customHeight="1">
       <c r="A13" t="s" s="11">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B13" s="12">
         <v>9527</v>
       </c>
-      <c r="C13" s="10"/>
+      <c r="C13" t="s" s="9">
+        <v>5</v>
+      </c>
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
       <c r="F13" s="14"/>
@@ -1848,20 +1861,24 @@
     </row>
     <row r="14" ht="20.35" customHeight="1">
       <c r="A14" t="s" s="11">
-        <v>18</v>
-      </c>
-      <c r="B14" t="s" s="12">
-        <v>19</v>
-      </c>
-      <c r="C14" s="14"/>
+        <v>20</v>
+      </c>
+      <c r="B14" s="12">
+        <v>9527</v>
+      </c>
+      <c r="C14" s="10"/>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
     </row>
     <row r="15" ht="20.35" customHeight="1">
-      <c r="A15" s="19"/>
-      <c r="B15" s="20"/>
+      <c r="A15" t="s" s="11">
+        <v>21</v>
+      </c>
+      <c r="B15" t="s" s="12">
+        <v>22</v>
+      </c>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
@@ -1930,6 +1947,15 @@
       <c r="E22" s="14"/>
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
+    </row>
+    <row r="23" ht="20.35" customHeight="1">
+      <c r="A23" s="19"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>